<commit_message>
tried to add validity checker for storage type.
</commit_message>
<xml_diff>
--- a/example_data/storages/storages-input.xlsx
+++ b/example_data/storages/storages-input.xlsx
@@ -238,16 +238,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -464,8 +468,8 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -534,6 +538,13 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L1001" type="list">
+      <formula1>"storage_investment_variable_type_continuous,storage_investment_variable_type_integer"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -557,186 +568,186 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="37.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="42.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>